<commit_message>
All data added to database.
</commit_message>
<xml_diff>
--- a/Backend/Excel/Final_12_month_enrollment_compiled.xlsx
+++ b/Backend/Excel/Final_12_month_enrollment_compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bipularyal/Desktop/FISK_IPDES_Proj/Backend/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345B1A2F-9B84-164D-B2E3-97C8ED4C33D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBB8417-DCC7-4D4F-AC0D-BF1F65D5A2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{EEB9D67A-3292-BA43-8182-FD9C08CD7949}"/>
   </bookViews>
@@ -38,24 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
-    <t>Total 12-month unduplicated headcount</t>
-  </si>
-  <si>
-    <t>Undergraduate student unduplicated headcount</t>
-  </si>
-  <si>
-    <t>Graduate student unduplicated headcount</t>
-  </si>
-  <si>
-    <t>Total 12-month full-time equivalent (FTE) student enrollment</t>
-  </si>
-  <si>
-    <t>Undergraduate student FTE</t>
-  </si>
-  <si>
-    <t>Graduate student FTE</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -174,6 +156,24 @@
   </si>
   <si>
     <t> 18</t>
+  </si>
+  <si>
+    <t>Total 12month unduplicated headcount</t>
+  </si>
+  <si>
+    <t>ug unduplicated headcount</t>
+  </si>
+  <si>
+    <t>g unduplicated headcount</t>
+  </si>
+  <si>
+    <t>Total 12month fte enrollment</t>
+  </si>
+  <si>
+    <t>ug FTE</t>
+  </si>
+  <si>
+    <t>g FTE</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,37 +554,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="I1" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="K1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -592,16 +592,16 @@
         <v>2010</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2">
         <v>677</v>
@@ -627,16 +627,16 @@
         <v>2011</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2">
         <v>629</v>
@@ -662,16 +662,16 @@
         <v>2012</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2">
         <v>563</v>
@@ -697,16 +697,16 @@
         <v>2013</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2">
         <v>643</v>
@@ -732,16 +732,16 @@
         <v>2014</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F6" s="2">
         <v>682</v>
@@ -767,16 +767,16 @@
         <v>2015</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2">
         <v>791</v>
@@ -802,16 +802,16 @@
         <v>2016</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2">
         <v>868</v>
@@ -837,16 +837,16 @@
         <v>2017</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2">
         <v>777</v>
@@ -872,10 +872,10 @@
         <v>2018</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2">
         <v>454</v>
@@ -907,16 +907,16 @@
         <v>2019</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F11" s="2">
         <v>800</v>

</xml_diff>